<commit_message>
Added column in QC Text.xlsx file
</commit_message>
<xml_diff>
--- a/QC Test.xlsx
+++ b/QC Test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\KAYESH\Source\Repos\IbneKayesh\Sieve.HR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Sheikh Asad Quadir\ASP.NET CORE\Kayes Vai\HR2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC50582B-EB55-4956-A496-E48BFA3902A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="855" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="855" windowWidth="20730" windowHeight="11040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Model</t>
   </si>
@@ -132,12 +131,15 @@
   </si>
   <si>
     <t>CompanyController</t>
+  </si>
+  <si>
+    <t>DropDown Select2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,14 +476,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,14 +567,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51677852-9C0A-46D4-AF5E-E7CE9FA057EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,14 +688,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA56E62B-C6FA-4AEB-BFB4-8659B5E2DC10}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,10 +710,11 @@
     <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -743,10 +746,13 @@
         <v>33</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -778,10 +784,13 @@
         <v>21</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -793,6 +802,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Duty and Top Bar
</commit_message>
<xml_diff>
--- a/QC Test.xlsx
+++ b/QC Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\KAYESH\Source\Repos\IbneKayesh\Sieve.HR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426BFD62-A3FB-4936-814F-E902366126BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80F2402-7699-406E-B337-615D0C2D1D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="855" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8220" yWindow="3045" windowWidth="20460" windowHeight="10770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="44">
   <si>
     <t>Model</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Index Page DisplayNameFor</t>
+  </si>
+  <si>
+    <t>HR_DUTY_ROSTER</t>
+  </si>
+  <si>
+    <t>DutyRosterController</t>
+  </si>
+  <si>
+    <t>DutyRoster</t>
   </si>
 </sst>
 </file>
@@ -495,10 +504,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,6 +600,32 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -602,10 +637,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,6 +773,44 @@
         <v>21</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -748,10 +821,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,6 +976,50 @@
         <v>21</v>
       </c>
     </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on Emp Education
</commit_message>
<xml_diff>
--- a/QC Test.xlsx
+++ b/QC Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="3045" windowWidth="20460" windowHeight="10770" activeTab="1"/>
+    <workbookView xWindow="8220" yWindow="3045" windowWidth="20460" windowHeight="10770"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="95">
   <si>
     <t>Model</t>
   </si>
@@ -659,8 +659,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,9 @@
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1022,8 +1024,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,12 +1263,24 @@
       <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1512,7 +1526,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,19 +1780,45 @@
       <c r="A8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">

</xml_diff>

<commit_message>
Working on HR attendance....
</commit_message>
<xml_diff>
--- a/QC Test.xlsx
+++ b/QC Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="3045" windowWidth="20460" windowHeight="10770" activeTab="1"/>
+    <workbookView xWindow="8220" yWindow="3045" windowWidth="20460" windowHeight="10770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="95">
   <si>
     <t>Model</t>
   </si>
@@ -660,7 +660,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,8 +1052,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,17 +1114,39 @@
       <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1557,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,10 +1648,18 @@
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>

</xml_diff>